<commit_message>
Individual Customer Data, edited
</commit_message>
<xml_diff>
--- a/Ind_Customer_Day.xlsx
+++ b/Ind_Customer_Day.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>An Individual Customer's usage on 2023-01-19</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>An Individual Customer's usage on 2023-01-20</t>
   </si>
   <si>
     <t>Time</t>
@@ -83,12 +83,6 @@
   </si>
   <si>
     <t>19:00:00</t>
-  </si>
-  <si>
-    <t>20:00:00</t>
-  </si>
-  <si>
-    <t>21:00:00</t>
   </si>
 </sst>
 </file>
@@ -434,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -468,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.009000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -476,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -508,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.0059983338</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -516,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1.6662E-06</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -540,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -548,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -564,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -572,7 +566,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -596,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.0249949995</v>
+        <v>0.0219958328</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -604,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.0210069444</v>
+        <v>0.0200061111</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -612,23 +606,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>